<commit_message>
Widened the Test Suite name column (B) to accommodate longer names
</commit_message>
<xml_diff>
--- a/templates/excel/full-template.xlsx
+++ b/templates/excel/full-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286515FD-5DD1-3A42-836F-9DAB4C359C99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD185A1F-0D3B-9147-9396-80A1B150106F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
@@ -2023,7 +2023,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="3" width="60.6640625" customWidth="1"/>
+    <col min="2" max="2" width="65.83203125" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>

</xml_diff>